<commit_message>
03.11.2024 - PART 1
</commit_message>
<xml_diff>
--- a/1__REPORT_AUTOMATION/XML_PROJECT/PROJECT_PART_1/ALFRED_AI/REFERENCE_FILES/FUNCTIONS.xlsx
+++ b/1__REPORT_AUTOMATION/XML_PROJECT/PROJECT_PART_1/ALFRED_AI/REFERENCE_FILES/FUNCTIONS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westhomas/Desktop/ALFRED/1__REPORT_AUTOMATION/XML_PROJECT/PROJECT_PART_1/PHASE 2 - Parsing and Identifying Excel Formulas/REFERENCE_FILES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/westhomas/Desktop/ALFRED/1__REPORT_AUTOMATION/XML_PROJECT/PROJECT_PART_1/ALFRED_AI/REFERENCE_FILES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964F2B05-4D1B-5446-A6E9-6A8966456565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF8E67A0-30FF-5C48-A1D1-08025AEAF03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="880" windowWidth="17380" windowHeight="22500" xr2:uid="{E496BFA4-66BC-49D0-9628-6D200FD426F9}"/>
+    <workbookView xWindow="1260" yWindow="880" windowWidth="34740" windowHeight="22500" xr2:uid="{E496BFA4-66BC-49D0-9628-6D200FD426F9}"/>
   </bookViews>
   <sheets>
     <sheet name="FUNCTIONS" sheetId="3" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="65">
   <si>
     <t>IF</t>
   </si>
@@ -223,6 +223,15 @@
   </si>
   <si>
     <t>['CONDITION']</t>
+  </si>
+  <si>
+    <t>IFNA</t>
+  </si>
+  <si>
+    <t>IFERROR</t>
+  </si>
+  <si>
+    <t>['CONDITION', 'CORRECTION']</t>
   </si>
 </sst>
 </file>
@@ -874,10 +883,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A235A256-1673-734F-BB7F-A0F53732F27F}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScale="107" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="107" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -935,6 +944,40 @@
         <v>8</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1021,7 +1064,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>